<commit_message>
Acrecentando Deep learning nas palavras chaves
</commit_message>
<xml_diff>
--- a/artigos_filtrados.xlsx
+++ b/artigos_filtrados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,16 +476,16 @@
         <v>2020</v>
       </c>
       <c r="E2" t="n">
-        <v>30.02110027855153</v>
+        <v>33.55299442896936</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Summer weather conditions influence winter survival of honey bees (Apis mellifera) in the northeastern United States</t>
+          <t>Tracking individual honeybees among wildflower clusters with computer vision-facilitated pollinator monitoring</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -495,35 +495,35 @@
         <v>2021</v>
       </c>
       <c r="E3" t="n">
-        <v>20.9199860724234</v>
+        <v>22.36274373259053</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The prediction of swarming in honeybee colonies using vibrational spectra</t>
+          <t>Summer weather conditions influence winter survival of honey bees (Apis mellifera) in the northeastern United States</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E4" t="n">
-        <v>12.26344011142061</v>
+        <v>22.36274373259053</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>IoT-Based Bee Swarm Activity Acoustic Classification Using Deep Neural Networks</t>
+          <t>Assessing the potential for deep learning and computer vision to identify bumble bee species from images</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -533,102 +533,102 @@
         <v>2021</v>
       </c>
       <c r="E5" t="n">
-        <v>10.28894150417827</v>
+        <v>16.9658077994429</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Assessing the potential for deep learning and computer vision to identify bumble bee species from images</t>
+          <t>The prediction of swarming in honeybee colonies using vibrational spectra</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E6" t="n">
-        <v>10.28894150417827</v>
+        <v>13.70619777158774</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Satisfiability Logic Analysis Via Radial Basis Function Neural Network with Artificial Bee Colony Algorithm</t>
+          <t>IoT-Based Bee Swarm Activity Acoustic Classification Using Deep Neural Networks</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
         <v>2021</v>
       </c>
       <c r="E7" t="n">
-        <v>8.652451253481896</v>
+        <v>10.72676880222841</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>274</v>
+        <v>228</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Markerless tracking of an entire honey bee colony</t>
+          <t>Satisfiability Logic Analysis Via Radial Basis Function Neural Network with Artificial Bee Colony Algorithm</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" t="n">
         <v>2021</v>
       </c>
       <c r="E8" t="n">
-        <v>7.015961002785517</v>
+        <v>9.020640668523679</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>401</v>
+        <v>274</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Automatic Data Clustering Based Mean Best Artificial Bee Colony Algorithm</t>
+          <t>Markerless tracking of an entire honey bee colony</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
         <v>2021</v>
       </c>
       <c r="E9" t="n">
-        <v>5.77374651810585</v>
+        <v>7.314512534818943</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>333</v>
+        <v>401</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A Novel Neural Network Training Algorithm for the Identification of Nonlinear Static Systems: Artificial Bee Colony Algorithm Based on Effective Scout Bee Stage</t>
+          <t>Automatic Data Clustering Based Mean Best Artificial Bee Colony Algorithm</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
         <v>2021</v>
       </c>
       <c r="E10" t="n">
-        <v>5.379470752089137</v>
+        <v>6.171935933147632</v>
       </c>
     </row>
     <row r="11">
@@ -647,64 +647,64 @@
         <v>2021</v>
       </c>
       <c r="E11" t="n">
-        <v>5.09682451253482</v>
+        <v>6.171935933147632</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Artificial Bee Colony Optimization Algorithm Incorporated With Fuzzy Theory for Real-Time Machine Learning Control of Articulated Robotic Manipulators</t>
+          <t>A Novel Neural Network Training Algorithm for the Identification of Nonlinear Static Systems: Artificial Bee Colony Algorithm Based on Effective Scout Bee Stage</t>
         </is>
       </c>
       <c r="C12" t="n">
         <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E12" t="n">
-        <v>4.86441504178273</v>
+        <v>5.608384401114207</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>169</v>
+        <v>332</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Artificial bee colony algorithm: A component-wise analysis using diversity measurement</t>
+          <t>Artificial Bee Colony Optimization Algorithm Incorporated With Fuzzy Theory for Real-Time Machine Learning Control of Articulated Robotic Manipulators</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
         <v>2020</v>
       </c>
       <c r="E13" t="n">
-        <v>4.313454038997214</v>
+        <v>5.436699164345404</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>411</v>
+        <v>169</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>An Improved Bees Algorithm for Training Deep Recurrent Networks for Sentiment Classification</t>
+          <t>Artificial bee colony algorithm: A component-wise analysis using diversity measurement</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D14" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E14" t="n">
-        <v>3.742980501392758</v>
+        <v>4.82091922005571</v>
       </c>
     </row>
     <row r="15">
@@ -723,54 +723,54 @@
         <v>2020</v>
       </c>
       <c r="E15" t="n">
-        <v>3.721532033426184</v>
+        <v>4.159359331476323</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>494</v>
+        <v>411</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Self-Powered Smart Beehive Monitoring and Control System (SBMaCS)</t>
+          <t>An Improved Bees Algorithm for Training Deep Recurrent Networks for Sentiment Classification</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
         <v>2021</v>
       </c>
       <c r="E16" t="n">
-        <v>3.249373259052925</v>
+        <v>3.902256267409471</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>496</v>
+        <v>231</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Audio, Image, Video, and Weather Datasets for Continuous Electronic Beehive Monitoring</t>
+          <t>An Efficient Intrusion Detection Model Based on Hybridization of Artificial Bee Colony and Dragonfly Algorithms for Training Multilayer Perceptrons</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E17" t="n">
-        <v>3.249373259052925</v>
+        <v>3.497799442896936</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>512</v>
+        <v>494</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Real-time monitoring of deformed wing virus-infected bee foraging behavior following histone deacetylase inhibitor treatment</t>
+          <t>Self-Powered Smart Beehive Monitoring and Control System (SBMaCS)</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -780,73 +780,73 @@
         <v>2021</v>
       </c>
       <c r="E18" t="n">
-        <v>3.249373259052925</v>
+        <v>3.473467966573816</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>519</v>
+        <v>496</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>An Optimized Neuro-Bee Algorithm Approach to Predict the FRP-Concrete Bond Strength of RC Beams</t>
+          <t>Audio, Image, Video, and Weather Datasets for Continuous Electronic Beehive Monitoring</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E19" t="n">
-        <v>3.249373259052925</v>
+        <v>3.473467966573816</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>231</v>
+        <v>512</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>An Efficient Intrusion Detection Model Based on Hybridization of Artificial Bee Colony and Dragonfly Algorithms for Training Multilayer Perceptrons</t>
+          <t>Real-time monitoring of deformed wing virus-infected bee foraging behavior following histone deacetylase inhibitor treatment</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E20" t="n">
-        <v>3.129610027855153</v>
+        <v>3.473467966573816</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>539</v>
+        <v>519</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Robust Queen Bee Assisted Genetic Algorithm (QBGA) Optimized Fractional Order PID (FOPID) Controller for Not Necessarily Minimum Phase Power Converters</t>
+          <t>An Optimized Neuro-Bee Algorithm Approach to Predict the FRP-Concrete Bond Strength of RC Beams</t>
         </is>
       </c>
       <c r="C21" t="n">
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E21" t="n">
-        <v>2.106490250696379</v>
+        <v>3.473467966573816</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>510</v>
+        <v>539</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Native bees in Mediterranean semi-arid agroecosystems: Unravelling the effects of biophysical habitat, floral resource, and honeybees</t>
+          <t>Robust Queen Bee Assisted Genetic Algorithm (QBGA) Optimized Fractional Order PID (FOPID) Controller for Not Necessarily Minimum Phase Power Converters</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -856,35 +856,35 @@
         <v>2021</v>
       </c>
       <c r="E22" t="n">
-        <v>2.106490250696379</v>
+        <v>2.196128133704736</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>645</v>
+        <v>510</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Edge-Based Detection of Varroosis in Beehives with IoT Devices with Embedded and TPU-Accelerated Machine Learning</t>
+          <t>Native bees in Mediterranean semi-arid agroecosystems: Unravelling the effects of biophysical habitat, floral resource, and honeybees</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
         <v>2021</v>
       </c>
       <c r="E23" t="n">
-        <v>0.7250000000000001</v>
+        <v>2.196128133704736</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Artificial Neural Networks Hidden Unit and Weight Connection Optimization by Quasi-Refection-Based Learning Artificial Bee Colony Algorithm</t>
+          <t>Edge-Based Detection of Varroosis in Beehives with IoT Devices with Embedded and TPU-Accelerated Machine Learning</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -894,16 +894,16 @@
         <v>2021</v>
       </c>
       <c r="E24" t="n">
-        <v>0.7250000000000001</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Proposed Smart Monitoring System for the Detection of Bee Swarming</t>
+          <t>Artificial Neural Networks Hidden Unit and Weight Connection Optimization by Quasi-Refection-Based Learning Artificial Bee Colony Algorithm</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -913,16 +913,16 @@
         <v>2021</v>
       </c>
       <c r="E25" t="n">
-        <v>0.7250000000000001</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>An Intelligent Monitoring System for Assessing Bee Hive Health</t>
+          <t>Proposed Smart Monitoring System for the Detection of Bee Swarming</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -932,16 +932,16 @@
         <v>2021</v>
       </c>
       <c r="E26" t="n">
-        <v>0.7250000000000001</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Acoustic Scene Classification and Visualization of Beehive Sounds Using Machine Learning Algorithms and Grad-CAM</t>
+          <t>An Intelligent Monitoring System for Assessing Bee Hive Health</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -951,54 +951,54 @@
         <v>2021</v>
       </c>
       <c r="E27" t="n">
-        <v>0.7250000000000001</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>AlexNet, AdaBoost and Artificial Bee Colony Based Hybrid Model for Electricity Theft Detection in Smart Grids</t>
+          <t>Acoustic Scene Classification and Visualization of Beehive Sounds Using Machine Learning Algorithms and Grad-CAM</t>
         </is>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7250000000000001</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>653</v>
+        <v>664</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Honey Bee Colony Population Daily Loss Rate Forecasting and an Early Warning Method Using Temporal Convolutional Networks</t>
+          <t>AlexNet, AdaBoost and Artificial Bee Colony Based Hybrid Model for Electricity Theft Detection in Smart Grids</t>
         </is>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E29" t="n">
-        <v>0.47</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>RFID Technology Serving Honey Bee Research: A Comprehensive Description of a 32-Antenna System to Study Honey Bee and Queen Behavior</t>
+          <t>Honey Bee Colony Population Daily Loss Rate Forecasting and an Early Warning Method Using Temporal Convolutional Networks</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1008,16 +1008,16 @@
         <v>2021</v>
       </c>
       <c r="E30" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DC model for SiC MOSFETs using artificial neural network optimized by artificial bee colony algorithm</t>
+          <t>RFID Technology Serving Honey Bee Research: A Comprehensive Description of a 32-Antenna System to Study Honey Bee and Queen Behavior</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1027,16 +1027,16 @@
         <v>2021</v>
       </c>
       <c r="E31" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Intrusion Detection for Network Based on Elite Clone Artificial Bee Colony and Back Propagation Neural Network</t>
+          <t>DC model for SiC MOSFETs using artificial neural network optimized by artificial bee colony algorithm</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1046,54 +1046,54 @@
         <v>2021</v>
       </c>
       <c r="E32" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Comparison of Feature Extraction Methods for Sound-Based Classification of Honey Bee Activity</t>
+          <t>Intrusion Detection for Network Based on Elite Clone Artificial Bee Colony and Back Propagation Neural Network</t>
         </is>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E33" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Energy-Efficient Wireless Weight Sensor for Remote Beehive Monitoring</t>
+          <t>Comparison of Feature Extraction Methods for Sound-Based Classification of Honey Bee Activity</t>
         </is>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E34" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>832</v>
+        <v>676</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Flow-mediated olfactory communication in honeybee swarms</t>
+          <t>Energy-Efficient Wireless Weight Sensor for Remote Beehive Monitoring</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1103,24 +1103,43 @@
         <v>2021</v>
       </c>
       <c r="E35" t="n">
-        <v>0.385</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
+        <v>832</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Flow-mediated olfactory communication in honeybee swarms</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.395</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
         <v>652</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>Application of artificial bee colony algorithm and back propagation neural network in color evaluation of human-machine interaction interfaces</t>
         </is>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="n">
-        <v>0.17</v>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="n">
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Acrecentando *computer vision nas keywords nível 5
</commit_message>
<xml_diff>
--- a/artigos_filtrados.xlsx
+++ b/artigos_filtrados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,16 +476,16 @@
         <v>2020</v>
       </c>
       <c r="E2" t="n">
-        <v>33.55299442896936</v>
+        <v>62.77777777777778</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tracking individual honeybees among wildflower clusters with computer vision-facilitated pollinator monitoring</t>
+          <t>Summer weather conditions influence winter survival of honey bees (Apis mellifera) in the northeastern United States</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -495,16 +495,16 @@
         <v>2021</v>
       </c>
       <c r="E3" t="n">
-        <v>22.36274373259053</v>
+        <v>51.11111111111111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Summer weather conditions influence winter survival of honey bees (Apis mellifera) in the northeastern United States</t>
+          <t>Tracking individual honeybees among wildflower clusters with computer vision-facilitated pollinator monitoring</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -514,7 +514,7 @@
         <v>2021</v>
       </c>
       <c r="E4" t="n">
-        <v>22.36274373259053</v>
+        <v>51.11111111111111</v>
       </c>
     </row>
     <row r="5">
@@ -533,7 +533,7 @@
         <v>2021</v>
       </c>
       <c r="E5" t="n">
-        <v>16.9658077994429</v>
+        <v>48.33333333333334</v>
       </c>
     </row>
     <row r="6">
@@ -552,73 +552,73 @@
         <v>2020</v>
       </c>
       <c r="E6" t="n">
-        <v>13.70619777158774</v>
+        <v>46.11111111111111</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>IoT-Based Bee Swarm Activity Acoustic Classification Using Deep Neural Networks</t>
+          <t>An Artificial Bee Colony Algorithm for Data Replication Optimization in Cloud Environments</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E7" t="n">
-        <v>10.72676880222841</v>
+        <v>46.11111111111111</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>228</v>
+        <v>332</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Satisfiability Logic Analysis Via Radial Basis Function Neural Network with Artificial Bee Colony Algorithm</t>
+          <t>Artificial Bee Colony Optimization Algorithm Incorporated With Fuzzy Theory for Real-Time Machine Learning Control of Articulated Robotic Manipulators</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E8" t="n">
-        <v>9.020640668523679</v>
+        <v>39.16666666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>274</v>
+        <v>340</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Markerless tracking of an entire honey bee colony</t>
+          <t>Visual Diagnosis of the Varroa Destructor Parasitic Mite in Honeybees Using Object Detector Techniques</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
         <v>2021</v>
       </c>
       <c r="E9" t="n">
-        <v>7.314512534818943</v>
+        <v>34.16666666666667</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Automatic Data Clustering Based Mean Best Artificial Bee Colony Algorithm</t>
+          <t>Detection of bee diseases with a hybrid deep learning method</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -628,16 +628,16 @@
         <v>2021</v>
       </c>
       <c r="E10" t="n">
-        <v>6.171935933147632</v>
+        <v>32.77777777777778</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Detection of bee diseases with a hybrid deep learning method</t>
+          <t>Automatic Data Clustering Based Mean Best Artificial Bee Colony Algorithm</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -647,396 +647,394 @@
         <v>2021</v>
       </c>
       <c r="E11" t="n">
-        <v>6.171935933147632</v>
+        <v>32.77777777777778</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>333</v>
+        <v>519</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A Novel Neural Network Training Algorithm for the Identification of Nonlinear Static Systems: Artificial Bee Colony Algorithm Based on Effective Scout Bee Stage</t>
+          <t>An Optimized Neuro-Bee Algorithm Approach to Predict the FRP-Concrete Bond Strength of RC Beams</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E12" t="n">
-        <v>5.608384401114207</v>
+        <v>31.38888888888889</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>332</v>
+        <v>512</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Artificial Bee Colony Optimization Algorithm Incorporated With Fuzzy Theory for Real-Time Machine Learning Control of Articulated Robotic Manipulators</t>
+          <t>Real-time monitoring of deformed wing virus-infected bee foraging behavior following histone deacetylase inhibitor treatment</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E13" t="n">
-        <v>5.436699164345404</v>
+        <v>31.38888888888889</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>169</v>
+        <v>494</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Artificial bee colony algorithm: A component-wise analysis using diversity measurement</t>
+          <t>Self-Powered Smart Beehive Monitoring and Control System (SBMaCS)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E14" t="n">
-        <v>4.82091922005571</v>
+        <v>31.38888888888889</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>193</v>
+        <v>496</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Precipitation forecast of the Wujiang River Basin based on artificial bee colony algorithm and backpropagation neural network</t>
+          <t>Audio, Image, Video, and Weather Datasets for Continuous Electronic Beehive Monitoring</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E15" t="n">
-        <v>4.159359331476323</v>
+        <v>31.38888888888889</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>411</v>
+        <v>648</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>An Improved Bees Algorithm for Training Deep Recurrent Networks for Sentiment Classification</t>
+          <t>Proposed Smart Monitoring System for the Detection of Bee Swarming</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>2021</v>
       </c>
       <c r="E16" t="n">
-        <v>3.902256267409471</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>231</v>
+        <v>645</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>An Efficient Intrusion Detection Model Based on Hybridization of Artificial Bee Colony and Dragonfly Algorithms for Training Multilayer Perceptrons</t>
+          <t>Edge-Based Detection of Varroosis in Beehives with IoT Devices with Embedded and TPU-Accelerated Machine Learning</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E17" t="n">
-        <v>3.497799442896936</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>494</v>
+        <v>664</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Self-Powered Smart Beehive Monitoring and Control System (SBMaCS)</t>
+          <t>AlexNet, AdaBoost and Artificial Bee Colony Based Hybrid Model for Electricity Theft Detection in Smart Grids</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E18" t="n">
-        <v>3.473467966573816</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>496</v>
+        <v>659</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Audio, Image, Video, and Weather Datasets for Continuous Electronic Beehive Monitoring</t>
+          <t>Acoustic Scene Classification and Visualization of Beehive Sounds Using Machine Learning Algorithms and Grad-CAM</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>2021</v>
       </c>
       <c r="E19" t="n">
-        <v>3.473467966573816</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>512</v>
+        <v>654</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Real-time monitoring of deformed wing virus-infected bee foraging behavior following histone deacetylase inhibitor treatment</t>
+          <t>AI-Driven Multiobjective Scheduling Algorithm of Flood Control Materials Based on Pareto Artificial Bee Colony</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>2021</v>
       </c>
       <c r="E20" t="n">
-        <v>3.473467966573816</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>519</v>
+        <v>649</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>An Optimized Neuro-Bee Algorithm Approach to Predict the FRP-Concrete Bond Strength of RC Beams</t>
+          <t>An Intelligent Monitoring System for Assessing Bee Hive Health</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E21" t="n">
-        <v>3.473467966573816</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>539</v>
+        <v>646</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Robust Queen Bee Assisted Genetic Algorithm (QBGA) Optimized Fractional Order PID (FOPID) Controller for Not Necessarily Minimum Phase Power Converters</t>
+          <t>Artificial Neural Networks Hidden Unit and Weight Connection Optimization by Quasi-Refection-Based Learning Artificial Bee Colony Algorithm</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>2021</v>
       </c>
       <c r="E22" t="n">
-        <v>2.196128133704736</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>510</v>
+        <v>192</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Native bees in Mediterranean semi-arid agroecosystems: Unravelling the effects of biophysical habitat, floral resource, and honeybees</t>
+          <t>IoT-Based Bee Swarm Activity Acoustic Classification Using Deep Neural Networks</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
         <v>2021</v>
       </c>
       <c r="E23" t="n">
-        <v>2.196128133704736</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>645</v>
+        <v>228</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Edge-Based Detection of Varroosis in Beehives with IoT Devices with Embedded and TPU-Accelerated Machine Learning</t>
+          <t>Satisfiability Logic Analysis Via Radial Basis Function Neural Network with Artificial Bee Colony Algorithm</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D24" t="n">
         <v>2021</v>
       </c>
       <c r="E24" t="n">
-        <v>0.775</v>
+        <v>28.16666666666667</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>646</v>
+        <v>274</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Artificial Neural Networks Hidden Unit and Weight Connection Optimization by Quasi-Refection-Based Learning Artificial Bee Colony Algorithm</t>
+          <t>Markerless tracking of an entire honey bee colony</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D25" t="n">
         <v>2021</v>
       </c>
       <c r="E25" t="n">
-        <v>0.775</v>
+        <v>27.33333333333333</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>648</v>
+        <v>169</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Proposed Smart Monitoring System for the Detection of Bee Swarming</t>
+          <t>Artificial bee colony algorithm: A component-wise analysis using diversity measurement</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D26" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E26" t="n">
-        <v>0.775</v>
+        <v>26.83333333333334</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>649</v>
+        <v>333</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>An Intelligent Monitoring System for Assessing Bee Hive Health</t>
+          <t>A Novel Neural Network Training Algorithm for the Identification of Nonlinear Static Systems: Artificial Bee Colony Algorithm Based on Effective Scout Bee Stage</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27" t="n">
         <v>2021</v>
       </c>
       <c r="E27" t="n">
-        <v>0.775</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>659</v>
+        <v>193</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Acoustic Scene Classification and Visualization of Beehive Sounds Using Machine Learning Algorithms and Grad-CAM</t>
+          <t>Precipitation forecast of the Wujiang River Basin based on artificial bee colony algorithm and backpropagation neural network</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E28" t="n">
-        <v>0.775</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>664</v>
+        <v>231</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>AlexNet, AdaBoost and Artificial Bee Colony Based Hybrid Model for Electricity Theft Detection in Smart Grids</t>
+          <t>An Efficient Intrusion Detection Model Based on Hybridization of Artificial Bee Colony and Dragonfly Algorithms for Training Multilayer Perceptrons</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D29" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="E29" t="n">
-        <v>0.775</v>
+        <v>25.16666666666667</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>653</v>
+        <v>411</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Honey Bee Colony Population Daily Loss Rate Forecasting and an Early Warning Method Using Temporal Convolutional Networks</t>
+          <t>An Improved Bees Algorithm for Training Deep Recurrent Networks for Sentiment Classification</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" t="n">
         <v>2021</v>
       </c>
       <c r="E30" t="n">
-        <v>0.49</v>
+        <v>19.66666666666666</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RFID Technology Serving Honey Bee Research: A Comprehensive Description of a 32-Antenna System to Study Honey Bee and Queen Behavior</t>
+          <t>Application of artificial bee colony algorithm and back propagation neural network in color evaluation of human-machine interaction interfaces</t>
         </is>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
-      <c r="D31" t="n">
-        <v>2021</v>
-      </c>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
-        <v>0.49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DC model for SiC MOSFETs using artificial neural network optimized by artificial bee colony algorithm</t>
+          <t>Honey Bee Colony Population Daily Loss Rate Forecasting and an Early Warning Method Using Temporal Convolutional Networks</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1046,16 +1044,16 @@
         <v>2021</v>
       </c>
       <c r="E32" t="n">
-        <v>0.49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Intrusion Detection for Network Based on Elite Clone Artificial Bee Colony and Back Propagation Neural Network</t>
+          <t>DC model for SiC MOSFETs using artificial neural network optimized by artificial bee colony algorithm</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1065,81 +1063,159 @@
         <v>2021</v>
       </c>
       <c r="E33" t="n">
-        <v>0.49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Comparison of Feature Extraction Methods for Sound-Based Classification of Honey Bee Activity</t>
+          <t>Intrusion Detection for Network Based on Elite Clone Artificial Bee Colony and Back Propagation Neural Network</t>
         </is>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E34" t="n">
-        <v>0.49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Energy-Efficient Wireless Weight Sensor for Remote Beehive Monitoring</t>
+          <t>Comparison of Feature Extraction Methods for Sound-Based Classification of Honey Bee Activity</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="E35" t="n">
-        <v>0.49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>832</v>
+        <v>539</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Flow-mediated olfactory communication in honeybee swarms</t>
+          <t>Robust Queen Bee Assisted Genetic Algorithm (QBGA) Optimized Fractional Order PID (FOPID) Controller for Not Necessarily Minimum Phase Power Converters</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="n">
         <v>2021</v>
       </c>
       <c r="E36" t="n">
-        <v>0.395</v>
+        <v>12.55555555555556</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>652</v>
+        <v>510</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Application of artificial bee colony algorithm and back propagation neural network in color evaluation of human-machine interaction interfaces</t>
+          <t>Native bees in Mediterranean semi-arid agroecosystems: Unravelling the effects of biophysical habitat, floral resource, and honeybees</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2021</v>
+      </c>
       <c r="E37" t="n">
-        <v>0.19</v>
+        <v>12.55555555555556</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>657</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>RFID Technology Serving Honey Bee Research: A Comprehensive Description of a 32-Antenna System to Study Honey Bee and Queen Behavior</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E38" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>676</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Energy-Efficient Wireless Weight Sensor for Remote Beehive Monitoring</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E39" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>495</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Week Ahead Electricity Price Forecasting Using Artificial Bee Colony Optimized Extreme Learning Machine with Wavelet Decomposition</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E40" t="n">
+        <v>6.277777777777778</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>832</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Flow-mediated olfactory communication in honeybee swarms</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E41" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>